<commit_message>
add RTS Lot 1 again
</commit_message>
<xml_diff>
--- a/tools/dora/RTS/RTS-DORA-ICT-related-incidents.xlsx
+++ b/tools/dora/RTS/RTS-DORA-ICT-related-incidents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imanabshirali/Desktop/stage MAi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4A8B6A-B9AD-6D46-961C-AF14AA4A5687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20765D5A-3EED-B646-B920-CD754D64AC01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17520" activeTab="1" xr2:uid="{07E11555-D7C4-E248-B1CA-88155D1FBDDE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" activeTab="1" xr2:uid="{07E11555-D7C4-E248-B1CA-88155D1FBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="2" r:id="rId1"/>
@@ -1486,8 +1486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B35FE3-E2E1-6544-BD94-781CE4F49196}">
   <dimension ref="A1:G694"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H86" sqref="H86"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="91" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D111" sqref="D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1518,8 +1518,7 @@
       <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="15" t="s">
+      <c r="C2" s="15" t="s">
         <v>43</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -1531,8 +1530,7 @@
       <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="15" t="s">
+      <c r="C3" s="15" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="6" t="s">
@@ -1623,8 +1621,7 @@
       <c r="B9" s="2">
         <v>2</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="15" t="s">
+      <c r="C9" s="15" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="6" t="s">
@@ -1726,8 +1723,7 @@
       <c r="B16" s="2">
         <v>2</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="15" t="s">
+      <c r="C16" s="15" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="6" t="s">
@@ -1807,8 +1803,7 @@
       <c r="B22" s="2">
         <v>2</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="15" t="s">
+      <c r="C22" s="15" t="s">
         <v>26</v>
       </c>
       <c r="E22" s="6" t="s">
@@ -1878,8 +1873,7 @@
       <c r="B27" s="2">
         <v>2</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="15" t="s">
+      <c r="C27" s="15" t="s">
         <v>4</v>
       </c>
       <c r="E27" s="6" t="s">
@@ -1964,8 +1958,7 @@
       <c r="B33" s="2">
         <v>2</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="15" t="s">
+      <c r="C33" s="15" t="s">
         <v>5</v>
       </c>
       <c r="E33" s="6" t="s">
@@ -2035,8 +2028,7 @@
       <c r="B38" s="2">
         <v>2</v>
       </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="15" t="s">
+      <c r="C38" s="15" t="s">
         <v>6</v>
       </c>
       <c r="E38" s="6" t="s">
@@ -2273,8 +2265,7 @@
       <c r="B54" s="2">
         <v>1</v>
       </c>
-      <c r="C54" s="3"/>
-      <c r="D54" s="15" t="s">
+      <c r="C54" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E54" s="6" t="s">
@@ -2286,8 +2277,7 @@
       <c r="B55" s="2">
         <v>2</v>
       </c>
-      <c r="C55" s="3"/>
-      <c r="D55" s="15" t="s">
+      <c r="C55" s="15" t="s">
         <v>7</v>
       </c>
       <c r="E55" s="6" t="s">
@@ -2430,8 +2420,7 @@
       <c r="B65" s="2">
         <v>2</v>
       </c>
-      <c r="C65" s="3"/>
-      <c r="D65" s="15" t="s">
+      <c r="C65" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E65" s="6" t="s">
@@ -2696,8 +2685,7 @@
       <c r="B83" s="2">
         <v>1</v>
       </c>
-      <c r="C83" s="3"/>
-      <c r="D83" s="15" t="s">
+      <c r="C83" s="15" t="s">
         <v>41</v>
       </c>
       <c r="E83" s="27" t="s">
@@ -2709,8 +2697,7 @@
       <c r="B84" s="2">
         <v>2</v>
       </c>
-      <c r="C84" s="3"/>
-      <c r="D84" s="15" t="s">
+      <c r="C84" s="15" t="s">
         <v>13</v>
       </c>
       <c r="E84" s="6" t="s">
@@ -2883,8 +2870,7 @@
       <c r="B96" s="2">
         <v>1</v>
       </c>
-      <c r="C96" s="3"/>
-      <c r="D96" s="15" t="s">
+      <c r="C96" s="15" t="s">
         <v>80</v>
       </c>
       <c r="E96" s="6" t="s">
@@ -2896,8 +2882,7 @@
       <c r="B97" s="2">
         <v>2</v>
       </c>
-      <c r="C97" s="3"/>
-      <c r="D97" s="15" t="s">
+      <c r="C97" s="15" t="s">
         <v>14</v>
       </c>
       <c r="E97" s="6" t="s">
@@ -2959,8 +2944,7 @@
       <c r="B102" s="2">
         <v>2</v>
       </c>
-      <c r="C102" s="3"/>
-      <c r="D102" s="15" t="s">
+      <c r="C102" s="15" t="s">
         <v>15</v>
       </c>
       <c r="E102" s="6" t="s">
@@ -2983,8 +2967,7 @@
       <c r="B104" s="2">
         <v>1</v>
       </c>
-      <c r="C104" s="3"/>
-      <c r="D104" s="15" t="s">
+      <c r="C104" s="15" t="s">
         <v>85</v>
       </c>
       <c r="E104" s="6" t="s">
@@ -2996,8 +2979,7 @@
       <c r="B105" s="2">
         <v>2</v>
       </c>
-      <c r="C105" s="3"/>
-      <c r="D105" s="3" t="s">
+      <c r="C105" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E105" s="6" t="s">

</xml_diff>